<commit_message>
Predictive and Prescriptive analytics
</commit_message>
<xml_diff>
--- a/Data/output.xlsx
+++ b/Data/output.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="98">
-  <si>
-    <t>Date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="100">
   <si>
     <t>Warehouse Code</t>
   </si>
@@ -71,6 +68,15 @@
   </si>
   <si>
     <t>CO2 Total</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Day</t>
   </si>
   <si>
     <t>WH NOIDA</t>
@@ -314,9 +320,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -369,12 +372,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,13 +671,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:22">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -733,1369 +735,1507 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:22">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>44205</v>
-      </c>
-      <c r="C2">
+      <c r="B2">
         <v>30447</v>
       </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="G2">
+        <v>201</v>
       </c>
       <c r="H2">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>21000061</v>
       </c>
       <c r="K2">
-        <v>21000061</v>
-      </c>
-      <c r="L2">
         <v>5</v>
       </c>
-      <c r="M2" t="s">
-        <v>78</v>
+      <c r="L2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2">
+        <v>0.02092</v>
       </c>
       <c r="N2">
-        <v>0.02092</v>
+        <v>400</v>
       </c>
       <c r="O2">
-        <v>400</v>
+        <v>8.368</v>
       </c>
       <c r="P2">
-        <v>8.368</v>
+        <v>0.161468928</v>
       </c>
       <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
         <v>0.161468928</v>
       </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
       <c r="T2">
-        <v>0.161468928</v>
+        <v>2021</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:22">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
-        <v>44215</v>
-      </c>
-      <c r="C3">
+      <c r="B3">
         <v>34192</v>
       </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="G3">
+        <v>194.1</v>
       </c>
       <c r="H3">
-        <v>194.1</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>20605097</v>
       </c>
       <c r="K3">
-        <v>20605097</v>
-      </c>
-      <c r="L3">
         <v>9</v>
       </c>
-      <c r="M3" t="s">
-        <v>79</v>
+      <c r="L3" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3">
+        <v>0.02219</v>
       </c>
       <c r="N3">
-        <v>0.02219</v>
+        <v>200</v>
       </c>
       <c r="O3">
-        <v>200</v>
+        <v>4.438000000000001</v>
       </c>
       <c r="P3">
-        <v>4.438000000000001</v>
+        <v>0.08269591680000002</v>
       </c>
       <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
         <v>0.08269591680000002</v>
       </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
       <c r="T3">
-        <v>0.08269591680000002</v>
+        <v>2021</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:22">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
-        <v>44238</v>
-      </c>
-      <c r="C4">
+      <c r="B4">
         <v>38454</v>
       </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>692</v>
       </c>
       <c r="J4">
-        <v>692</v>
+        <v>20478515</v>
       </c>
       <c r="K4">
-        <v>20478515</v>
-      </c>
-      <c r="L4">
         <v>5</v>
       </c>
-      <c r="M4" t="s">
-        <v>80</v>
+      <c r="L4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M4">
+        <v>0.019</v>
       </c>
       <c r="N4">
-        <v>0.019</v>
+        <v>960</v>
       </c>
       <c r="O4">
-        <v>960</v>
+        <v>18.24</v>
       </c>
       <c r="P4">
-        <v>18.24</v>
+        <v>0</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>26.506368</v>
       </c>
       <c r="S4">
         <v>26.506368</v>
       </c>
       <c r="T4">
-        <v>26.506368</v>
+        <v>2021</v>
+      </c>
+      <c r="U4">
+        <v>2</v>
+      </c>
+      <c r="V4">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:22">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
-        <v>44268</v>
-      </c>
-      <c r="C5">
+      <c r="B5">
         <v>30492</v>
       </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="G5">
+        <v>362.4</v>
       </c>
       <c r="H5">
-        <v>362.4</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>20761978</v>
       </c>
       <c r="K5">
-        <v>20761978</v>
-      </c>
-      <c r="L5">
         <v>7</v>
       </c>
-      <c r="M5" t="s">
-        <v>81</v>
+      <c r="L5" t="s">
+        <v>83</v>
+      </c>
+      <c r="M5">
+        <v>0.04767</v>
       </c>
       <c r="N5">
-        <v>0.04767</v>
+        <v>96</v>
       </c>
       <c r="O5">
-        <v>96</v>
+        <v>4.57632</v>
       </c>
       <c r="P5">
-        <v>4.57632</v>
+        <v>0.159212003328</v>
       </c>
       <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
         <v>0.159212003328</v>
       </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
       <c r="T5">
-        <v>0.159212003328</v>
+        <v>2021</v>
+      </c>
+      <c r="U5">
+        <v>3</v>
+      </c>
+      <c r="V5">
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:22">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
-        <v>44274</v>
-      </c>
-      <c r="C6">
+      <c r="B6">
         <v>39040</v>
       </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>182</v>
       </c>
       <c r="I6">
-        <v>182</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>20930844</v>
       </c>
       <c r="K6">
-        <v>20930844</v>
-      </c>
-      <c r="L6">
         <v>6</v>
       </c>
-      <c r="M6" t="s">
-        <v>82</v>
+      <c r="L6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M6">
+        <v>0.0915</v>
       </c>
       <c r="N6">
-        <v>0.0915</v>
+        <v>375</v>
       </c>
       <c r="O6">
-        <v>375</v>
+        <v>34.3125</v>
       </c>
       <c r="P6">
-        <v>34.3125</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>0.1748565</v>
       </c>
       <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
         <v>0.1748565</v>
       </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
       <c r="T6">
-        <v>0.1748565</v>
+        <v>2021</v>
+      </c>
+      <c r="U6">
+        <v>3</v>
+      </c>
+      <c r="V6">
+        <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:22">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
-        <v>44279</v>
-      </c>
-      <c r="C7">
+      <c r="B7">
         <v>31163</v>
       </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="G7">
+        <v>199.4</v>
       </c>
       <c r="H7">
-        <v>199.4</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>20203383</v>
       </c>
       <c r="K7">
-        <v>20203383</v>
-      </c>
-      <c r="L7">
         <v>3</v>
       </c>
-      <c r="M7" t="s">
-        <v>83</v>
+      <c r="L7" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7">
+        <v>0.02219</v>
       </c>
       <c r="N7">
-        <v>0.02219</v>
+        <v>500</v>
       </c>
       <c r="O7">
-        <v>500</v>
+        <v>11.095</v>
       </c>
       <c r="P7">
-        <v>11.095</v>
+        <v>0.212384928</v>
       </c>
       <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
         <v>0.212384928</v>
       </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
       <c r="T7">
-        <v>0.212384928</v>
+        <v>2021</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="V7">
+        <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:22">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
-        <v>44288</v>
-      </c>
-      <c r="C8">
+      <c r="B8">
         <v>37518</v>
       </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="G8">
+        <v>505.7</v>
       </c>
       <c r="H8">
-        <v>505.7</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>20387569</v>
       </c>
       <c r="K8">
-        <v>20387569</v>
-      </c>
-      <c r="L8">
         <v>9</v>
       </c>
-      <c r="M8" t="s">
-        <v>84</v>
+      <c r="L8" t="s">
+        <v>86</v>
+      </c>
+      <c r="M8">
+        <v>0.019</v>
       </c>
       <c r="N8">
-        <v>0.019</v>
+        <v>1120</v>
       </c>
       <c r="O8">
-        <v>1120</v>
+        <v>21.28</v>
       </c>
       <c r="P8">
-        <v>21.28</v>
+        <v>1.033084416</v>
       </c>
       <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
         <v>1.033084416</v>
       </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
       <c r="T8">
-        <v>1.033084416</v>
+        <v>2021</v>
+      </c>
+      <c r="U8">
+        <v>4</v>
+      </c>
+      <c r="V8">
+        <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:22">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
-        <v>44318</v>
-      </c>
-      <c r="C9">
+      <c r="B9">
         <v>32188</v>
       </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="G9">
+        <v>350.6</v>
       </c>
       <c r="H9">
-        <v>350.6</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>20258239</v>
       </c>
       <c r="K9">
-        <v>20258239</v>
-      </c>
-      <c r="L9">
         <v>1</v>
       </c>
-      <c r="M9" t="s">
-        <v>85</v>
+      <c r="L9" t="s">
+        <v>87</v>
+      </c>
+      <c r="M9">
+        <v>0.032</v>
       </c>
       <c r="N9">
-        <v>0.032</v>
+        <v>250</v>
       </c>
       <c r="O9">
-        <v>250</v>
+        <v>8</v>
       </c>
       <c r="P9">
-        <v>8</v>
+        <v>0.2692608</v>
       </c>
       <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
         <v>0.2692608</v>
       </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
       <c r="T9">
-        <v>0.2692608</v>
+        <v>2021</v>
+      </c>
+      <c r="U9">
+        <v>5</v>
+      </c>
+      <c r="V9">
+        <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:22">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
-        <v>44335</v>
-      </c>
-      <c r="C10">
+      <c r="B10">
         <v>38258</v>
       </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>331.9</v>
       </c>
       <c r="J10">
-        <v>331.9</v>
+        <v>20623857</v>
       </c>
       <c r="K10">
-        <v>20623857</v>
-      </c>
-      <c r="L10">
         <v>2</v>
       </c>
-      <c r="M10" t="s">
-        <v>86</v>
+      <c r="L10" t="s">
+        <v>88</v>
+      </c>
+      <c r="M10">
+        <v>0.03392</v>
       </c>
       <c r="N10">
-        <v>0.03392</v>
+        <v>2240</v>
       </c>
       <c r="O10">
-        <v>2240</v>
+        <v>75.9808</v>
       </c>
       <c r="P10">
-        <v>75.9808</v>
+        <v>0</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>52.957857792</v>
       </c>
       <c r="S10">
         <v>52.957857792</v>
       </c>
       <c r="T10">
-        <v>52.957857792</v>
+        <v>2021</v>
+      </c>
+      <c r="U10">
+        <v>5</v>
+      </c>
+      <c r="V10">
+        <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:22">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
-        <v>44385</v>
-      </c>
-      <c r="C11">
+      <c r="B11">
         <v>35553</v>
       </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>581.3</v>
       </c>
       <c r="J11">
-        <v>581.3</v>
+        <v>20611749</v>
       </c>
       <c r="K11">
-        <v>20611749</v>
-      </c>
-      <c r="L11">
         <v>1</v>
       </c>
-      <c r="M11" t="s">
-        <v>87</v>
+      <c r="L11" t="s">
+        <v>89</v>
+      </c>
+      <c r="M11">
+        <v>16.53807</v>
       </c>
       <c r="N11">
-        <v>16.53807</v>
+        <v>128</v>
       </c>
       <c r="O11">
-        <v>128</v>
+        <v>2116.87296</v>
       </c>
       <c r="P11">
-        <v>2116.87296</v>
+        <v>0</v>
       </c>
       <c r="Q11">
         <v>0</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>2584.1303284608</v>
       </c>
       <c r="S11">
         <v>2584.1303284608</v>
       </c>
       <c r="T11">
-        <v>2584.1303284608</v>
+        <v>2021</v>
+      </c>
+      <c r="U11">
+        <v>7</v>
+      </c>
+      <c r="V11">
+        <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:22">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
-        <v>44433</v>
-      </c>
-      <c r="C12">
+      <c r="B12">
         <v>32992</v>
       </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>724.1</v>
       </c>
       <c r="J12">
-        <v>724.1</v>
+        <v>20416356</v>
       </c>
       <c r="K12">
-        <v>20416356</v>
-      </c>
-      <c r="L12">
         <v>8</v>
       </c>
-      <c r="M12" t="s">
-        <v>88</v>
+      <c r="L12" t="s">
+        <v>90</v>
+      </c>
+      <c r="M12">
+        <v>0.019</v>
       </c>
       <c r="N12">
-        <v>0.019</v>
+        <v>560</v>
       </c>
       <c r="O12">
-        <v>560</v>
+        <v>10.64</v>
       </c>
       <c r="P12">
-        <v>10.64</v>
+        <v>0</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>16.1792904</v>
       </c>
       <c r="S12">
         <v>16.1792904</v>
       </c>
       <c r="T12">
-        <v>16.1792904</v>
+        <v>2021</v>
+      </c>
+      <c r="U12">
+        <v>8</v>
+      </c>
+      <c r="V12">
+        <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:22">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
-        <v>44434</v>
-      </c>
-      <c r="C13">
+      <c r="B13">
         <v>35240</v>
       </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="G13">
+        <v>560.7</v>
       </c>
       <c r="H13">
-        <v>560.7</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>20727111</v>
       </c>
       <c r="K13">
-        <v>20727111</v>
-      </c>
-      <c r="L13">
         <v>4</v>
       </c>
-      <c r="M13" t="s">
-        <v>89</v>
+      <c r="L13" t="s">
+        <v>91</v>
+      </c>
+      <c r="M13">
+        <v>0.0184</v>
       </c>
       <c r="N13">
-        <v>0.0184</v>
+        <v>1120</v>
       </c>
       <c r="O13">
-        <v>1120</v>
+        <v>20.608</v>
       </c>
       <c r="P13">
-        <v>20.608</v>
+        <v>1.1092709376</v>
       </c>
       <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
         <v>1.1092709376</v>
       </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
       <c r="T13">
-        <v>1.1092709376</v>
+        <v>2021</v>
+      </c>
+      <c r="U13">
+        <v>8</v>
+      </c>
+      <c r="V13">
+        <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:22">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
-        <v>44450</v>
-      </c>
-      <c r="C14">
+      <c r="B14">
         <v>39526</v>
       </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>158.2</v>
       </c>
       <c r="I14">
-        <v>158.2</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>20258208</v>
       </c>
       <c r="K14">
-        <v>20258208</v>
-      </c>
-      <c r="L14">
         <v>4</v>
       </c>
-      <c r="M14" t="s">
-        <v>90</v>
+      <c r="L14" t="s">
+        <v>92</v>
+      </c>
+      <c r="M14">
+        <v>0.032</v>
       </c>
       <c r="N14">
-        <v>0.032</v>
+        <v>400</v>
       </c>
       <c r="O14">
-        <v>400</v>
+        <v>12.8</v>
       </c>
       <c r="P14">
-        <v>12.8</v>
+        <v>0</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>0.05669888000000001</v>
       </c>
       <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
         <v>0.05669888000000001</v>
       </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
       <c r="T14">
-        <v>0.05669888000000001</v>
+        <v>2021</v>
+      </c>
+      <c r="U14">
+        <v>9</v>
+      </c>
+      <c r="V14">
+        <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:22">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
-        <v>44460</v>
-      </c>
-      <c r="C15">
+      <c r="B15">
         <v>35508</v>
       </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>653.8</v>
       </c>
       <c r="I15">
-        <v>653.8</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>20663620</v>
       </c>
       <c r="K15">
-        <v>20663620</v>
-      </c>
-      <c r="L15">
         <v>3</v>
       </c>
-      <c r="M15" t="s">
-        <v>91</v>
+      <c r="L15" t="s">
+        <v>93</v>
+      </c>
+      <c r="M15">
+        <v>0.054</v>
       </c>
       <c r="N15">
-        <v>0.054</v>
+        <v>576</v>
       </c>
       <c r="O15">
-        <v>576</v>
+        <v>31.104</v>
       </c>
       <c r="P15">
-        <v>31.104</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>0.5694022656</v>
       </c>
       <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
         <v>0.5694022656</v>
       </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
       <c r="T15">
-        <v>0.5694022656</v>
+        <v>2021</v>
+      </c>
+      <c r="U15">
+        <v>9</v>
+      </c>
+      <c r="V15">
+        <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:22">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
-        <v>44460</v>
-      </c>
-      <c r="C16">
+      <c r="B16">
         <v>39434</v>
       </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+      <c r="G16">
+        <v>275</v>
       </c>
       <c r="H16">
-        <v>275</v>
+        <v>0</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>20425836</v>
       </c>
       <c r="K16">
-        <v>20425836</v>
-      </c>
-      <c r="L16">
         <v>1</v>
       </c>
-      <c r="M16" t="s">
-        <v>92</v>
+      <c r="L16" t="s">
+        <v>94</v>
+      </c>
+      <c r="M16">
+        <v>0.022</v>
       </c>
       <c r="N16">
-        <v>0.022</v>
+        <v>560</v>
       </c>
       <c r="O16">
-        <v>560</v>
+        <v>12.32</v>
       </c>
       <c r="P16">
-        <v>12.32</v>
+        <v>0.325248</v>
       </c>
       <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
         <v>0.325248</v>
       </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
       <c r="T16">
-        <v>0.325248</v>
+        <v>2021</v>
+      </c>
+      <c r="U16">
+        <v>9</v>
+      </c>
+      <c r="V16">
+        <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:22">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="2">
-        <v>44461</v>
-      </c>
-      <c r="C17">
+      <c r="B17">
         <v>34395</v>
       </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" t="s">
-        <v>74</v>
+        <v>76</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>507.1</v>
       </c>
       <c r="J17">
-        <v>507.1</v>
+        <v>20679193</v>
       </c>
       <c r="K17">
-        <v>20679193</v>
-      </c>
-      <c r="L17">
         <v>1</v>
       </c>
-      <c r="M17" t="s">
-        <v>87</v>
+      <c r="L17" t="s">
+        <v>89</v>
+      </c>
+      <c r="M17">
+        <v>16.53807</v>
       </c>
       <c r="N17">
-        <v>16.53807</v>
+        <v>153</v>
       </c>
       <c r="O17">
-        <v>153</v>
+        <v>2530.32471</v>
       </c>
       <c r="P17">
-        <v>2530.32471</v>
+        <v>0</v>
       </c>
       <c r="Q17">
         <v>0</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>2694.5680869261</v>
       </c>
       <c r="S17">
         <v>2694.5680869261</v>
       </c>
       <c r="T17">
-        <v>2694.5680869261</v>
+        <v>2021</v>
+      </c>
+      <c r="U17">
+        <v>9</v>
+      </c>
+      <c r="V17">
+        <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:22">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
-        <v>44478</v>
-      </c>
-      <c r="C18">
+      <c r="B18">
         <v>33322</v>
       </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>617.9</v>
       </c>
       <c r="I18">
-        <v>617.9</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>20609480</v>
       </c>
       <c r="K18">
-        <v>20609480</v>
-      </c>
-      <c r="L18">
         <v>7</v>
       </c>
-      <c r="M18" t="s">
-        <v>93</v>
+      <c r="L18" t="s">
+        <v>95</v>
+      </c>
+      <c r="M18">
+        <v>0.0178</v>
       </c>
       <c r="N18">
-        <v>0.0178</v>
+        <v>560</v>
       </c>
       <c r="O18">
-        <v>560</v>
+        <v>9.968</v>
       </c>
       <c r="P18">
-        <v>9.968</v>
+        <v>0</v>
       </c>
       <c r="Q18">
-        <v>0</v>
+        <v>0.1724583616</v>
       </c>
       <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
         <v>0.1724583616</v>
       </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
       <c r="T18">
-        <v>0.1724583616</v>
+        <v>2021</v>
+      </c>
+      <c r="U18">
+        <v>10</v>
+      </c>
+      <c r="V18">
+        <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:22">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="2">
-        <v>44494</v>
-      </c>
-      <c r="C19">
+      <c r="B19">
         <v>37552</v>
       </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="G19">
+        <v>353.59</v>
       </c>
       <c r="H19">
-        <v>353.59</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>1010.2</v>
       </c>
       <c r="J19">
-        <v>1010.2</v>
+        <v>20344993</v>
       </c>
       <c r="K19">
-        <v>20344993</v>
-      </c>
-      <c r="L19">
         <v>6</v>
       </c>
-      <c r="M19" t="s">
-        <v>80</v>
+      <c r="L19" t="s">
+        <v>82</v>
+      </c>
+      <c r="M19">
+        <v>0.019</v>
       </c>
       <c r="N19">
-        <v>0.019</v>
+        <v>300</v>
       </c>
       <c r="O19">
-        <v>300</v>
+        <v>5.7</v>
       </c>
       <c r="P19">
-        <v>5.7</v>
+        <v>0.193484448</v>
       </c>
       <c r="Q19">
-        <v>0.193484448</v>
+        <v>0</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>12.092094</v>
       </c>
       <c r="S19">
-        <v>12.092094</v>
+        <v>12.285578448</v>
       </c>
       <c r="T19">
-        <v>12.285578448</v>
+        <v>2021</v>
+      </c>
+      <c r="U19">
+        <v>10</v>
+      </c>
+      <c r="V19">
+        <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:22">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="2">
-        <v>44515</v>
-      </c>
-      <c r="C20">
+      <c r="B20">
         <v>37518</v>
       </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="G20">
+        <v>505.7</v>
       </c>
       <c r="H20">
-        <v>505.7</v>
+        <v>0</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>20247100</v>
       </c>
       <c r="K20">
-        <v>20247100</v>
-      </c>
-      <c r="L20">
         <v>1</v>
       </c>
-      <c r="M20" t="s">
-        <v>94</v>
+      <c r="L20" t="s">
+        <v>96</v>
+      </c>
+      <c r="M20">
+        <v>56.584</v>
       </c>
       <c r="N20">
-        <v>56.584</v>
+        <v>2</v>
       </c>
       <c r="O20">
-        <v>2</v>
+        <v>113.168</v>
       </c>
       <c r="P20">
-        <v>113.168</v>
+        <v>5.4939895296</v>
       </c>
       <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
         <v>5.4939895296</v>
       </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
       <c r="T20">
-        <v>5.4939895296</v>
+        <v>2021</v>
+      </c>
+      <c r="U20">
+        <v>11</v>
+      </c>
+      <c r="V20">
+        <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:22">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="2">
-        <v>44543</v>
-      </c>
-      <c r="C21">
+      <c r="B21">
         <v>30977</v>
       </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>770.1</v>
       </c>
       <c r="I21">
-        <v>770.1</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>20203388</v>
       </c>
       <c r="K21">
-        <v>20203388</v>
-      </c>
-      <c r="L21">
         <v>2</v>
       </c>
-      <c r="M21" t="s">
-        <v>95</v>
+      <c r="L21" t="s">
+        <v>97</v>
+      </c>
+      <c r="M21">
+        <v>0.02219</v>
       </c>
       <c r="N21">
-        <v>0.02219</v>
+        <v>500</v>
       </c>
       <c r="O21">
-        <v>500</v>
+        <v>11.095</v>
       </c>
       <c r="P21">
-        <v>11.095</v>
+        <v>0</v>
       </c>
       <c r="Q21">
-        <v>0</v>
+        <v>0.239239266</v>
       </c>
       <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
         <v>0.239239266</v>
       </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
       <c r="T21">
-        <v>0.239239266</v>
+        <v>2021</v>
+      </c>
+      <c r="U21">
+        <v>12</v>
+      </c>
+      <c r="V21">
+        <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:22">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="2">
-        <v>44544</v>
-      </c>
-      <c r="C22">
+      <c r="B22">
         <v>32515</v>
       </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
-      </c>
-      <c r="G22" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>266.8</v>
       </c>
       <c r="I22">
-        <v>266.8</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>20733009</v>
       </c>
       <c r="K22">
-        <v>20733009</v>
-      </c>
-      <c r="L22">
         <v>8</v>
       </c>
-      <c r="M22" t="s">
-        <v>96</v>
+      <c r="L22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M22">
+        <v>0.04304</v>
       </c>
       <c r="N22">
-        <v>0.04304</v>
+        <v>125</v>
       </c>
       <c r="O22">
-        <v>125</v>
+        <v>5.38</v>
       </c>
       <c r="P22">
-        <v>5.38</v>
+        <v>0</v>
       </c>
       <c r="Q22">
-        <v>0</v>
+        <v>0.04019075200000001</v>
       </c>
       <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
         <v>0.04019075200000001</v>
       </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
       <c r="T22">
-        <v>0.04019075200000001</v>
+        <v>2021</v>
+      </c>
+      <c r="U22">
+        <v>12</v>
+      </c>
+      <c r="V22">
+        <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:22">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="2">
-        <v>44544</v>
-      </c>
-      <c r="C23">
+      <c r="B23">
         <v>37518</v>
       </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="F23" t="s">
-        <v>45</v>
-      </c>
-      <c r="G23" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="G23">
+        <v>505.7</v>
       </c>
       <c r="H23">
-        <v>505.7</v>
+        <v>0</v>
       </c>
       <c r="I23">
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>20549626</v>
       </c>
       <c r="K23">
-        <v>20549626</v>
-      </c>
-      <c r="L23">
         <v>51</v>
       </c>
-      <c r="M23" t="s">
-        <v>97</v>
+      <c r="L23" t="s">
+        <v>99</v>
+      </c>
+      <c r="M23">
+        <v>0.024</v>
       </c>
       <c r="N23">
-        <v>0.024</v>
+        <v>25</v>
       </c>
       <c r="O23">
-        <v>25</v>
+        <v>0.6</v>
       </c>
       <c r="P23">
-        <v>0.6</v>
+        <v>0.02912832</v>
       </c>
       <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
         <v>0.02912832</v>
       </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
       <c r="T23">
-        <v>0.02912832</v>
+        <v>2021</v>
+      </c>
+      <c r="U23">
+        <v>12</v>
+      </c>
+      <c r="V23">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>